<commit_message>
Update transmission line cost calculation
</commit_message>
<xml_diff>
--- a/InputData/Transmission/AC_Cables_Param.xlsx
+++ b/InputData/Transmission/AC_Cables_Param.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\OceanPortfolioOptimization\OceanPortfolioOptimization\InputData\Transmission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9851BC78-C720-424C-9771-A48457E2ED76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E151DCF3-74D2-4439-9DD2-8A7D3578C572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="4980" windowWidth="28800" windowHeight="15435" xr2:uid="{0AB40103-AD55-49E7-8440-AA1F2C5CDA15}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="21600" windowHeight="11385" xr2:uid="{0AB40103-AD55-49E7-8440-AA1F2C5CDA15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,9 +78,6 @@
     <t>Cable Cost [$/m]</t>
   </si>
   <si>
-    <t xml:space="preserve"> Cooper</t>
-  </si>
-  <si>
     <t>Aluminium</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>MVA Capacity</t>
+  </si>
+  <si>
+    <t>Copper</t>
   </si>
 </sst>
 </file>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9C025EC-B1B5-408F-B821-E4293B499EEF}">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I39" sqref="I2:I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,13 +489,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -537,7 +537,7 @@
         <v>176.59454624354933</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -567,7 +567,7 @@
         <v>198.99812604164649</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -597,7 +597,7 @@
         <v>220.35437132244917</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -627,7 +627,7 @@
         <v>250.44714729881716</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -657,7 +657,7 @@
         <v>295.70342012626793</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -687,7 +687,7 @@
         <v>338.46017116846667</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -717,7 +717,7 @@
         <v>396.65724431057026</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -747,7 +747,7 @@
         <v>469.39845196322995</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -777,7 +777,7 @@
         <v>546.84774563826875</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -807,7 +807,7 @@
         <v>635.68462492159176</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -837,7 +837,7 @@
         <v>719.61500834854837</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -867,7 +867,7 @@
         <v>330.2646285440112</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -897,7 +897,7 @@
         <v>398.32499038759329</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -927,7 +927,7 @@
         <v>457.15953784582916</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -957,7 +957,7 @@
         <v>530.39994927202156</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -987,7 +987,7 @@
         <v>613.12141231307919</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1017,7 +1017,7 @@
         <v>692.72843251169729</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1047,7 +1047,7 @@
         <v>775.58513635815916</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1077,7 +1077,7 @@
         <v>847.21033115055798</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1107,7 +1107,7 @@
         <v>426.32081805232497</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1137,7 +1137,7 @@
         <v>513.04748818479447</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1167,7 +1167,7 @@
         <v>588.56933355833053</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1197,7 +1197,7 @@
         <v>683.27598858051169</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1227,7 +1227,7 @@
         <v>791.13841890483764</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1257,7 +1257,7 @@
         <v>895.80817426816293</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1287,7 +1287,7 @@
         <v>1005.6259771412242</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1317,7 +1317,7 @@
         <v>1101.2556504028958</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1347,7 +1347,7 @@
         <v>612.5304027484965</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1377,7 +1377,7 @@
         <v>703.21431389580971</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1407,7 +1407,7 @@
         <v>817.62018251258996</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1437,7 +1437,7 @@
         <v>948.81056027130035</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1467,7 +1467,7 @@
         <v>1076.9883408407791</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1497,7 +1497,7 @@
         <v>1212.3537439181214</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1527,7 +1527,7 @@
         <v>1330.9389006669521</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1557,7 +1557,7 @@
         <v>988.88227969482091</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1587,7 +1587,7 @@
         <v>1079.6219400401878</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1617,7 +1617,7 @@
         <v>1174.4118526022389</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -1647,7 +1647,7 @@
         <v>1256.6275778097929</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -1677,7 +1677,7 @@
         <v>144.28802734618168</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1707,7 +1707,7 @@
         <v>158.60355428367794</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -1737,7 +1737,7 @@
         <v>176.59454624354933</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -1767,7 +1767,7 @@
         <v>196.08435952531934</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -1797,7 +1797,7 @@
         <v>226.776683117278</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -1827,7 +1827,7 @@
         <v>257.56539768896522</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -1857,7 +1857,7 @@
         <v>299.76251943689613</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -1887,7 +1887,7 @@
         <v>347.61384893991533</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -1917,7 +1917,7 @@
         <v>407.15681284882692</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -1947,7 +1947,7 @@
         <v>475.45454477058388</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -1977,7 +1977,7 @@
         <v>553.79428265786839</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -2007,7 +2007,7 @@
         <v>238.39017832928016</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2037,7 +2037,7 @@
         <v>291.80228771834095</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2067,7 +2067,7 @@
         <v>341.41976075288312</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2097,7 +2097,7 @@
         <v>404.12056358542122</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2127,7 +2127,7 @@
         <v>469.16368314216243</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2157,7 +2157,7 @@
         <v>542.89412264098542</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2187,7 +2187,7 @@
         <v>619.63435452984959</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2217,7 +2217,7 @@
         <v>699.50724326328282</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2247,7 +2247,7 @@
         <v>310.37189053139787</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2277,7 +2277,7 @@
         <v>377.62019955263918</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2307,7 +2307,7 @@
         <v>440.48764943923288</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -2337,7 +2337,7 @@
         <v>520.46442513951183</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -2367,7 +2367,7 @@
         <v>604.03969822087242</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -2397,7 +2397,7 @@
         <v>699.50724326328282</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -2427,7 +2427,7 @@
         <v>799.67023691747499</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -2457,7 +2457,7 @@
         <v>904.75961879393162</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -2487,7 +2487,7 @@
         <v>451.18741670290615</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -2517,7 +2517,7 @@
         <v>525.87723076665407</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -2547,7 +2547,7 @@
         <v>621.41438353090712</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -2577,7 +2577,7 @@
         <v>721.85113322380175</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -2607,7 +2607,7 @@
         <v>837.30206925774064</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -2637,7 +2637,7 @@
         <v>959.22696468389722</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -2667,7 +2667,7 @@
         <v>1087.9888494754523</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -2697,7 +2697,7 @@
         <v>825.66026346714852</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -2727,7 +2727,7 @@
         <v>909.11435176472901</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -2757,7 +2757,7 @@
         <v>996.29349374701746</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -2787,7 +2787,7 @@
         <v>1087.3639607763525</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>